<commit_message>
create and edit verification form added,
</commit_message>
<xml_diff>
--- a/temp/verification_form.xlsx
+++ b/temp/verification_form.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
   <si>
     <t>NO</t>
   </si>
@@ -40,13 +40,13 @@
     <t>سکونت اصلی</t>
   </si>
   <si>
-    <t>تمکی</t>
+    <t>ورقه</t>
   </si>
   <si>
     <t>قره باغ</t>
   </si>
   <si>
-    <t>کابل</t>
+    <t>کاپیسا</t>
   </si>
   <si>
     <t>اسم پدر</t>
@@ -58,10 +58,10 @@
     <t>سکونت فعلی</t>
   </si>
   <si>
-    <t>ویانا</t>
-  </si>
-  <si>
-    <t>امریکا</t>
+    <t>برلین</t>
+  </si>
+  <si>
+    <t>آلبانی</t>
   </si>
   <si>
     <t>اسم پدر کلان</t>
@@ -100,25 +100,22 @@
     <t>شغل</t>
   </si>
   <si>
-    <t>انجنیر نرم افزار</t>
-  </si>
-  <si>
     <t>رنگ چشم</t>
   </si>
   <si>
-    <t>سبز</t>
+    <t>Eyes Color</t>
   </si>
   <si>
     <t>مدت اقامت در خارج</t>
   </si>
   <si>
-    <t>4 سال</t>
+    <t>8 سال</t>
   </si>
   <si>
     <t>رنگ پوست</t>
   </si>
   <si>
-    <t>سفید</t>
+    <t>Skin Color</t>
   </si>
   <si>
     <t>تاریخ آخرین برگشت به افغانستان</t>
@@ -127,40 +124,34 @@
     <t>رنگ مو</t>
   </si>
   <si>
-    <t>سیاه</t>
+    <t>Hair Color</t>
   </si>
   <si>
     <t>شماره تماس در خارج</t>
   </si>
   <si>
-    <t>09388758943</t>
-  </si>
-  <si>
     <t>سایر علایم</t>
   </si>
   <si>
-    <t>working fine</t>
+    <t>Other Information</t>
   </si>
   <si>
     <t>ایمیل آدرس شخص متقاضی</t>
   </si>
   <si>
-    <t>a.gulistani@mfa.af</t>
-  </si>
-  <si>
     <t>اسم و شماره تماس وکیل/نماینده متقاضی در افغانستان</t>
   </si>
   <si>
-    <t>احمد فلانی گک قربان</t>
-  </si>
-  <si>
-    <t>988390403434</t>
+    <t>Delegate Name Delegate Last Name</t>
+  </si>
+  <si>
+    <t>Delegate Contact No. 1</t>
   </si>
   <si>
     <t>نوع خدمات</t>
   </si>
   <si>
-    <t>تذکره مثنی غیر حضوری</t>
+    <t>اخذ تذکره مثنی غیر حضوری</t>
   </si>
   <si>
     <t>در صورت مثنی دلیل آن نشانی شود</t>
@@ -169,19 +160,20 @@
     <t>شهرت و مشخصات تذکره اقارب اصولی (پدر، پدرکلان، برادر، کاکا و پسر کاکا) متقاضی</t>
   </si>
   <si>
-    <t>شمسیه احمدی</t>
-  </si>
-  <si>
-    <t>کامل</t>
-  </si>
-  <si>
-    <t>بنیاد</t>
+    <t>جلال الدین برخی تمنا</t>
+  </si>
+  <si>
+    <t>Siblings Father Name</t>
+  </si>
+  <si>
+    <t>Siblings Grand Father Name</t>
   </si>
   <si>
     <t>نوع قرابت</t>
   </si>
   <si>
-    <t>خواهر</t>
+    <t xml:space="preserve">پدر
+</t>
   </si>
   <si>
     <t>مشخصات تذکره</t>
@@ -1833,7 +1825,7 @@
         <v>13</v>
       </c>
       <c r="J6" s="7">
-        <v>7864</v>
+        <v>568956</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>14</v>
@@ -1904,7 +1896,7 @@
         <v>23</v>
       </c>
       <c r="I9" s="11">
-        <v>12</v>
+        <v>569</v>
       </c>
       <c r="J9" s="45" t="s">
         <v>24</v>
@@ -1922,19 +1914,17 @@
       <c r="C10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>27</v>
-      </c>
+      <c r="D10" s="19"/>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="4">
         <v>20</v>
       </c>
       <c r="H10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>29</v>
       </c>
       <c r="J10" s="45"/>
       <c r="K10" s="46"/>
@@ -1946,10 +1936,10 @@
         <v>7</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>31</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
@@ -1957,10 +1947,10 @@
         <v>21</v>
       </c>
       <c r="H11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="J11" s="45"/>
       <c r="K11" s="46"/>
@@ -1972,10 +1962,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="19">
-        <v>2012</v>
+        <v>4095</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
@@ -1983,10 +1973,10 @@
         <v>22</v>
       </c>
       <c r="H12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>36</v>
       </c>
       <c r="J12" s="45"/>
       <c r="K12" s="46"/>
@@ -1998,21 +1988,19 @@
         <v>9</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>38</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="4">
         <v>23</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J13" s="45"/>
       <c r="K13" s="46"/>
@@ -2023,25 +2011,23 @@
         <v>10</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>42</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D14" s="19"/>
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="4">
         <v>24</v>
       </c>
       <c r="H14" s="47" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I14" s="48"/>
       <c r="J14" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:17" customHeight="1" ht="21.75">
@@ -2050,10 +2036,10 @@
         <v>11</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="25"/>
@@ -2069,7 +2055,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
@@ -2083,7 +2069,7 @@
     <row r="17" spans="1:17" customHeight="1" ht="16.5">
       <c r="A17" s="18"/>
       <c r="B17" s="20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -2104,7 +2090,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
@@ -2115,7 +2101,7 @@
         <v>10</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
@@ -2129,7 +2115,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
@@ -2137,10 +2123,10 @@
         <v>26</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
@@ -2151,37 +2137,37 @@
         <v>15</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D20" s="9">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E20" s="9">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="F20" s="9">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G20" s="4">
         <v>27</v>
       </c>
       <c r="H20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" s="4">
+        <v>2132</v>
+      </c>
+      <c r="J20" s="4">
+        <v>123</v>
+      </c>
+      <c r="K20" s="4">
         <v>56</v>
-      </c>
-      <c r="I20" s="4">
-        <v>1994</v>
-      </c>
-      <c r="J20" s="4">
-        <v>5</v>
-      </c>
-      <c r="K20" s="4">
-        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:17" customHeight="1" ht="12.75">
       <c r="A21" s="18"/>
       <c r="B21" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C21" s="35"/>
       <c r="D21" s="35"/>
@@ -2221,7 +2207,7 @@
     </row>
     <row r="24" spans="1:17" customHeight="1" ht="15.75">
       <c r="B24" s="32" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>

</xml_diff>